<commit_message>
Project turnin Wk 2 update
changed a file name, updated main tracking sheet
</commit_message>
<xml_diff>
--- a/Time Tracking/CEIS400-MainTimeSheet-GroupC-22924.xlsx
+++ b/Time Tracking/CEIS400-MainTimeSheet-GroupC-22924.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d037e0306ecfb5d/Desktop/repos_cloned_here/silver-goggles/Time Tracking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d037e0306ecfb5d/Desktop/repos_cloned_here_laptop/silver-goggles/Time Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40B25DE9-E00C-4BC7-AF93-526C168704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{40B25DE9-E00C-4BC7-AF93-526C168704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9B7A971-D9FC-4E58-91B3-FF5DD30C3455}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-11820" windowWidth="16500" windowHeight="10875" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14445" yWindow="-12810" windowWidth="13845" windowHeight="10785" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member One" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Member Five'!$A$1:$E$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Member Four'!$A$1:$E$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Member One'!$A$1:$E$69</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Member Three'!$A$1:$E$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Member Three'!$A$1:$E$69</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Member Two'!$A$1:$E$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -172,6 +172,42 @@
   </si>
   <si>
     <t>Overall, I carefully went over every part of the test plan to make sure it was clear, comprehensive, and in line with the criteria and goals of the project. I also took into account potential hazards and backup plans to lessen any negative effects on the testing procedure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status Update Meeting – Confirming Individual Lab Assignments, Covering questions as necessary. </t>
+  </si>
+  <si>
+    <t>Laid foundation for VOPC matrix, gathered resources in order to complete assignment</t>
+  </si>
+  <si>
+    <t>Completed VOPC matrix.</t>
+  </si>
+  <si>
+    <t>Researched SQL educational videos to share with team for a refresher on the subject.</t>
+  </si>
+  <si>
+    <t>Began and Completed Class Diagram.</t>
+  </si>
+  <si>
+    <t>Initial assignments and meeting planning</t>
+  </si>
+  <si>
+    <t>Meeting one, going over GitHub Desktop - new tool</t>
+  </si>
+  <si>
+    <t>Meeting two, answering questions about project, assisting for turnins</t>
+  </si>
+  <si>
+    <t>Collating data for final turn in for this week</t>
+  </si>
+  <si>
+    <t>Downloaded Visio, watched live lesson and worked on assignment</t>
+  </si>
+  <si>
+    <t>Team Meeting, GitHub Desktop new tool</t>
+  </si>
+  <si>
+    <t>Struggled getting class diagram started, started and finished use case diagram</t>
   </si>
 </sst>
 </file>
@@ -239,7 +275,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -652,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -767,6 +809,18 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,10 +837,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1081,8 +1131,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1259,10 +1309,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="17">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1271,50 +1321,80 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="15">
+        <v>45355</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.8125</v>
+      </c>
       <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="11"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="15">
+        <v>45357</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.8125</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>45359</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.8125</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.875</v>
+      </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="11"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="15">
+        <v>45361</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0.875</v>
+      </c>
       <c r="C18" s="14"/>
       <c r="D18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="11"/>
+        <v>-0.875</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="17">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1604,9 +1684,9 @@
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
-      <c r="D47" s="7" t="str">
+      <c r="D47" s="7" t="e">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
-        <v>0:6:45</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E47" s="3"/>
     </row>
@@ -1638,8 +1718,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1732,10 +1812,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17">
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -1800,10 +1880,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="17">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1811,35 +1891,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>45358</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="11"/>
+        <v>0.10416666666666674</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="15">
+        <v>45359</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.8125</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.84375</v>
+      </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>45360</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.625</v>
+      </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="11"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
@@ -1852,10 +1956,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="17">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2147,7 +2251,7 @@
       <c r="C47" s="22"/>
       <c r="D47" s="7" t="str">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
-        <v>0:2:30</v>
+        <v>0:9:45</v>
       </c>
       <c r="E47" s="3"/>
     </row>
@@ -2177,10 +2281,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2273,10 +2377,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17">
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -2312,7 +2416,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D11" s="17">
-        <f t="shared" ref="D11:D46" si="0">(C11-B11)</f>
+        <f t="shared" ref="D11:D47" si="0">(C11-B11)</f>
         <v>5.208333333333337E-2</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -2348,10 +2452,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="17">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2359,67 +2463,107 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>45357</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>45358</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="11"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="15">
+        <v>45359</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.875</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>45360</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="11"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="15">
+        <v>45360</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0.65625</v>
+      </c>
       <c r="D19" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="19" t="s">
+        <f t="shared" ref="D19" si="1">(C19-B19)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -2429,7 +2573,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
@@ -2459,19 +2603,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
@@ -2511,19 +2655,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
@@ -2563,9 +2707,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
@@ -2575,7 +2717,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="19" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
@@ -2615,7 +2759,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="19"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
@@ -2625,7 +2769,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
@@ -2677,32 +2821,42 @@
       </c>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
       <c r="D46" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="1:5" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="16"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="12"/>
+    </row>
+    <row r="48" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="7" t="str">
-        <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
-        <v>2:2:15</v>
-      </c>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="7" t="str">
+        <f>TEXT(SUM(D9:D47), "d:h:mm")</f>
+        <v>2:6:20</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E3"/>
@@ -2727,8 +2881,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" activeCellId="1" sqref="B10 E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2821,10 +2975,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17">
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -2881,10 +3035,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="17">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2933,10 +3087,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="17">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3260,8 +3414,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3354,10 +3508,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17">
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -3422,10 +3576,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="17">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3482,10 +3636,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="17">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added missing Wk 1 files and wk 2 turn in
Added:
- WBS from MS project to group one, planning update soon to week 2 metrics
- Week 2 .zip for turnin
- use cases document from week 1
</commit_message>
<xml_diff>
--- a/Time Tracking/CEIS400-MainTimeSheet-GroupC-22924.xlsx
+++ b/Time Tracking/CEIS400-MainTimeSheet-GroupC-22924.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d037e0306ecfb5d/Desktop/repos_cloned_here_laptop/silver-goggles/Time Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{40B25DE9-E00C-4BC7-AF93-526C168704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9B7A971-D9FC-4E58-91B3-FF5DD30C3455}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{40B25DE9-E00C-4BC7-AF93-526C168704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A3F0A87-52C5-4E0A-831D-DAC820C67F61}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="-12810" windowWidth="13845" windowHeight="10785" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14700" yWindow="-15105" windowWidth="13845" windowHeight="10785" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member One" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Struggled getting class diagram started, started and finished use case diagram</t>
+  </si>
+  <si>
+    <t>Week 2 project – Use case descriptions.</t>
+  </si>
+  <si>
+    <t>Week 2 Project – Use case descriptions</t>
   </si>
 </sst>
 </file>
@@ -750,6 +756,18 @@
     <xf numFmtId="2" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -809,18 +827,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,6 +843,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1147,65 +1157,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1309,10 +1319,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1391,10 +1401,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1679,11 +1689,11 @@
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="7" t="e">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
         <v>#VALUE!</v>
@@ -1734,65 +1744,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1812,10 +1822,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="43">
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -1880,10 +1890,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1956,10 +1966,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2244,11 +2254,11 @@
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="7" t="str">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
         <v>0:9:45</v>
@@ -2299,65 +2309,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -2377,10 +2387,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="43">
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -2452,10 +2462,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2554,10 +2564,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="43">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2606,10 +2616,10 @@
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2658,10 +2668,10 @@
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2842,11 +2852,11 @@
       <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="7" t="str">
         <f>TEXT(SUM(D9:D47), "d:h:mm")</f>
         <v>2:6:20</v>
@@ -2882,7 +2892,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2897,65 +2907,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -2975,10 +2985,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="43">
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -3035,10 +3045,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3047,24 +3057,40 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="15">
+        <v>45358</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="11"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="15">
+        <v>45361</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.625</v>
+      </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="11"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
@@ -3087,10 +3113,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3375,14 +3401,14 @@
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="7" t="str">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
-        <v>0:3:00</v>
+        <v>0:6:00</v>
       </c>
       <c r="E47" s="3"/>
     </row>
@@ -3430,65 +3456,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -3508,10 +3534,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="43">
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23">
         <f>(C9-B9)</f>
         <v>0</v>
       </c>
@@ -3576,10 +3602,10 @@
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3636,10 +3662,10 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3924,11 +3950,11 @@
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="7" t="str">
         <f>TEXT(SUM(D9:D46), "d:h:mm")</f>
         <v>0:3:30</v>

</xml_diff>